<commit_message>
some docs for esinf functions
</commit_message>
<xml_diff>
--- a/src/src/main/resources/Legacy_Data.xlsx
+++ b/src/src/main/resources/Legacy_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miguel/Documents/2Year/LAPR3/sem3pi2023_24_g104/src/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C3BF85-66C0-164E-B8E2-6637E070441E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B650F685-5E0F-9642-81B4-8D7727A7897C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{ACBD79A1-D35B-4D3E-A78E-4F35CA726952}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{ACBD79A1-D35B-4D3E-A78E-4F35CA726952}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantas" sheetId="1" r:id="rId1"/>
@@ -42,8 +42,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1502" uniqueCount="259">
   <si>
     <t>Espécie</t>
   </si>
@@ -817,6 +839,9 @@
   </si>
   <si>
     <t>Semeadura</t>
+  </si>
+  <si>
+    <t>Area</t>
   </si>
 </sst>
 </file>
@@ -876,7 +901,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -887,7 +912,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1204,7 +1228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA74F46-7FB7-481B-9DAE-CE325D568C4A}">
   <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
@@ -3952,10 +3976,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{246DE277-EC3F-46EA-8D39-A978B7AEA5AE}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3966,7 +3990,7 @@
     <col min="5" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>176</v>
       </c>
@@ -3994,8 +4018,11 @@
       <c r="I1" s="2" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>101</v>
       </c>
@@ -4023,8 +4050,12 @@
       <c r="I2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" t="str">
+        <f>IF(D2=$D$12,1," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>101</v>
       </c>
@@ -4052,8 +4083,12 @@
       <c r="I3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J27" si="0">IF(D3=$D$12,1," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>101</v>
       </c>
@@ -4081,8 +4116,12 @@
       <c r="I4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>101</v>
       </c>
@@ -4110,8 +4149,12 @@
       <c r="I5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>103</v>
       </c>
@@ -4139,8 +4182,12 @@
       <c r="I6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>103</v>
       </c>
@@ -4168,8 +4215,12 @@
       <c r="I7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>103</v>
       </c>
@@ -4197,8 +4248,12 @@
       <c r="I8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>103</v>
       </c>
@@ -4226,8 +4281,12 @@
       <c r="I9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>103</v>
       </c>
@@ -4255,8 +4314,12 @@
       <c r="I10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>103</v>
       </c>
@@ -4284,8 +4347,12 @@
       <c r="I11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>102</v>
       </c>
@@ -4310,8 +4377,16 @@
       <c r="I12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12" cm="1">
+        <f t="array" ref="J12">IF(_xlfn.IFS(H12="un",G12*6*7.5),G12*6*7.5," ")</f>
+        <v>1350</v>
+      </c>
+      <c r="K12">
+        <f>J12/10000</f>
+        <v>0.13500000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>102</v>
       </c>
@@ -4336,8 +4411,16 @@
       <c r="I13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13" cm="1">
+        <f t="array" ref="J13">IF(_xlfn.IFS(H13="un",G13*5*5),G13*6*7.5," ")</f>
+        <v>900</v>
+      </c>
+      <c r="K13">
+        <f t="shared" ref="K13:K28" si="1">J13/10000</f>
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>106</v>
       </c>
@@ -4365,8 +4448,12 @@
       <c r="I14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>106</v>
       </c>
@@ -4394,8 +4481,12 @@
       <c r="I15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>106</v>
       </c>
@@ -4423,8 +4514,12 @@
       <c r="I16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>106</v>
       </c>
@@ -4452,8 +4547,12 @@
       <c r="I17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>106</v>
       </c>
@@ -4481,8 +4580,12 @@
       <c r="I18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>106</v>
       </c>
@@ -4510,8 +4613,12 @@
       <c r="I19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>106</v>
       </c>
@@ -4539,8 +4646,12 @@
       <c r="I20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>106</v>
       </c>
@@ -4568,8 +4679,12 @@
       <c r="I21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>106</v>
       </c>
@@ -4597,8 +4712,12 @@
       <c r="I22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J22" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>104</v>
       </c>
@@ -4623,8 +4742,16 @@
       <c r="I23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J23" cm="1">
+        <f t="array" ref="J23">IF(_xlfn.IFS(H23="un",G23*5*5),G23*5*5," ")</f>
+        <v>2250</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="1"/>
+        <v>0.22500000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>104</v>
       </c>
@@ -4649,8 +4776,16 @@
       <c r="I24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J24" cm="1">
+        <f t="array" ref="J24">IF(_xlfn.IFS(H24="un",G24*5*5),G24*5*5," ")</f>
+        <v>1500</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="1"/>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>104</v>
       </c>
@@ -4675,8 +4810,16 @@
       <c r="I25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J25" cm="1">
+        <f t="array" ref="J25">IF(_xlfn.IFS(H25="un",G25*5*5),G25*5*5," ")</f>
+        <v>1000</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>104</v>
       </c>
@@ -4701,8 +4844,16 @@
       <c r="I26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J26" cm="1">
+        <f t="array" ref="J26">IF(_xlfn.IFS(H26="un",G26*5*5),G26*5*5," ")</f>
+        <v>750</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="1"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>107</v>
       </c>
@@ -4727,8 +4878,15 @@
       <c r="I27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J27">
+        <v>1000</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>107</v>
       </c>
@@ -4752,6 +4910,13 @@
       </c>
       <c r="I28">
         <v>27</v>
+      </c>
+      <c r="J28">
+        <v>1400</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="1"/>
+        <v>0.14000000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -4768,14 +4933,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8273E431-88A0-4D26-AA21-9E0D94FE2923}">
   <dimension ref="A1:Q141"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A99" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" customWidth="1"/>
     <col min="5" max="5" width="28.6640625" bestFit="1" customWidth="1"/>
@@ -4794,7 +4959,7 @@
       <c r="A1" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" t="s">
         <v>178</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -4832,7 +4997,7 @@
       <c r="A2">
         <v>102</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" t="s">
         <v>181</v>
       </c>
       <c r="C2" t="s">
@@ -4873,7 +5038,7 @@
       <c r="A3">
         <v>102</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" t="s">
         <v>181</v>
       </c>
       <c r="C3" t="s">
@@ -4914,7 +5079,7 @@
       <c r="A4">
         <v>104</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" t="s">
         <v>183</v>
       </c>
       <c r="C4" t="s">
@@ -4955,7 +5120,7 @@
       <c r="A5">
         <v>104</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" t="s">
         <v>183</v>
       </c>
       <c r="C5" t="s">
@@ -4996,7 +5161,7 @@
       <c r="A6">
         <v>104</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" t="s">
         <v>183</v>
       </c>
       <c r="C6" t="s">
@@ -5037,7 +5202,7 @@
       <c r="A7">
         <v>102</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" t="s">
         <v>181</v>
       </c>
       <c r="C7" t="s">
@@ -5078,7 +5243,7 @@
       <c r="A8">
         <v>102</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" t="s">
         <v>181</v>
       </c>
       <c r="C8" t="s">
@@ -5119,7 +5284,7 @@
       <c r="A9">
         <v>102</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" t="s">
         <v>181</v>
       </c>
       <c r="C9" t="s">
@@ -5174,7 +5339,7 @@
       <c r="A10">
         <v>102</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" t="s">
         <v>181</v>
       </c>
       <c r="C10" t="s">
@@ -5229,7 +5394,7 @@
       <c r="A11">
         <v>104</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" t="s">
         <v>183</v>
       </c>
       <c r="C11" t="s">
@@ -5270,7 +5435,7 @@
       <c r="A12">
         <v>104</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" t="s">
         <v>183</v>
       </c>
       <c r="C12" t="s">
@@ -5311,7 +5476,7 @@
       <c r="A13">
         <v>104</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" t="s">
         <v>183</v>
       </c>
       <c r="C13" t="s">
@@ -5352,7 +5517,7 @@
       <c r="A14">
         <v>107</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" t="s">
         <v>246</v>
       </c>
       <c r="C14" t="s">
@@ -5393,7 +5558,7 @@
       <c r="A15">
         <v>107</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" t="s">
         <v>246</v>
       </c>
       <c r="C15" t="s">
@@ -5434,7 +5599,7 @@
       <c r="A16">
         <v>104</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" t="s">
         <v>183</v>
       </c>
       <c r="C16" t="s">
@@ -5489,7 +5654,7 @@
       <c r="A17">
         <v>104</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" t="s">
         <v>183</v>
       </c>
       <c r="C17" t="s">
@@ -5544,7 +5709,7 @@
       <c r="A18">
         <v>104</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" t="s">
         <v>183</v>
       </c>
       <c r="C18" t="s">
@@ -5599,7 +5764,7 @@
       <c r="A19">
         <v>102</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" t="s">
         <v>181</v>
       </c>
       <c r="C19" t="s">
@@ -5640,7 +5805,7 @@
       <c r="A20">
         <v>102</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" t="s">
         <v>181</v>
       </c>
       <c r="C20" t="s">
@@ -5681,7 +5846,7 @@
       <c r="A21">
         <v>104</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" t="s">
         <v>183</v>
       </c>
       <c r="C21" t="s">
@@ -5722,7 +5887,7 @@
       <c r="A22">
         <v>107</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" t="s">
         <v>246</v>
       </c>
       <c r="C22" t="s">
@@ -5763,7 +5928,7 @@
       <c r="A23">
         <v>107</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" t="s">
         <v>246</v>
       </c>
       <c r="C23" t="s">
@@ -5804,7 +5969,7 @@
       <c r="A24">
         <v>104</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" t="s">
         <v>183</v>
       </c>
       <c r="C24" t="s">
@@ -5845,7 +6010,7 @@
       <c r="A25">
         <v>104</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" t="s">
         <v>183</v>
       </c>
       <c r="C25" t="s">
@@ -5886,7 +6051,7 @@
       <c r="A26">
         <v>104</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" t="s">
         <v>183</v>
       </c>
       <c r="C26" t="s">
@@ -5927,7 +6092,7 @@
       <c r="A27">
         <v>107</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" t="s">
         <v>246</v>
       </c>
       <c r="C27" t="s">
@@ -5975,7 +6140,7 @@
       <c r="A28">
         <v>107</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" t="s">
         <v>246</v>
       </c>
       <c r="C28" t="s">
@@ -6023,7 +6188,7 @@
       <c r="A29">
         <v>104</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" t="s">
         <v>183</v>
       </c>
       <c r="C29" t="s">
@@ -6070,7 +6235,7 @@
         <v>Insert into culturaOperacaoFatorProducao (operacaofatorproducao,cultura) values (28,22);</v>
       </c>
       <c r="Q29" t="str">
-        <f t="shared" ref="Q27:Q31" si="13">"insert into Operacao"&amp;L29&amp;" (id,modo) values ("&amp;K29&amp;",(select id from modo where modo like '"&amp;D29&amp;"'));"</f>
+        <f t="shared" ref="Q29:Q31" si="13">"insert into Operacao"&amp;L29&amp;" (id,modo) values ("&amp;K29&amp;",(select id from modo where modo like '"&amp;D29&amp;"'));"</f>
         <v>insert into OperacaoFertilizacao (id,modo) values (28,(select id from modo where modo like 'Solo'));</v>
       </c>
     </row>
@@ -6078,7 +6243,7 @@
       <c r="A30">
         <v>104</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" t="s">
         <v>183</v>
       </c>
       <c r="C30" t="s">
@@ -6133,7 +6298,7 @@
       <c r="A31">
         <v>104</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" t="s">
         <v>183</v>
       </c>
       <c r="C31" t="s">
@@ -6188,7 +6353,7 @@
       <c r="A32">
         <v>102</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" t="s">
         <v>181</v>
       </c>
       <c r="C32" t="s">
@@ -6229,7 +6394,7 @@
       <c r="A33">
         <v>102</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" t="s">
         <v>181</v>
       </c>
       <c r="C33" t="s">
@@ -6270,7 +6435,7 @@
       <c r="A34">
         <v>107</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" t="s">
         <v>246</v>
       </c>
       <c r="C34" t="s">
@@ -6311,7 +6476,7 @@
       <c r="A35">
         <v>107</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" t="s">
         <v>246</v>
       </c>
       <c r="C35" t="s">
@@ -6352,7 +6517,7 @@
       <c r="A36">
         <v>107</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" t="s">
         <v>246</v>
       </c>
       <c r="C36" t="s">
@@ -6400,7 +6565,7 @@
       <c r="A37">
         <v>107</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" t="s">
         <v>246</v>
       </c>
       <c r="C37" t="s">
@@ -6448,7 +6613,7 @@
       <c r="A38">
         <v>106</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" t="s">
         <v>220</v>
       </c>
       <c r="C38" t="s">
@@ -6488,7 +6653,7 @@
       <c r="A39">
         <v>103</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" t="s">
         <v>182</v>
       </c>
       <c r="C39" t="s">
@@ -6533,7 +6698,7 @@
       <c r="A40">
         <v>106</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" t="s">
         <v>220</v>
       </c>
       <c r="C40" t="s">
@@ -6574,7 +6739,7 @@
       <c r="A41">
         <v>106</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B41" t="s">
         <v>220</v>
       </c>
       <c r="C41" t="s">
@@ -6615,7 +6780,7 @@
       <c r="A42">
         <v>106</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" t="s">
         <v>220</v>
       </c>
       <c r="C42" t="s">
@@ -6655,7 +6820,7 @@
       <c r="A43">
         <v>103</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" t="s">
         <v>182</v>
       </c>
       <c r="C43" t="s">
@@ -6696,7 +6861,7 @@
       <c r="A44">
         <v>106</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B44" t="s">
         <v>220</v>
       </c>
       <c r="C44" t="s">
@@ -6737,7 +6902,7 @@
       <c r="A45">
         <v>106</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B45" t="s">
         <v>220</v>
       </c>
       <c r="C45" t="s">
@@ -6778,7 +6943,7 @@
       <c r="A46">
         <v>106</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B46" t="s">
         <v>220</v>
       </c>
       <c r="C46" t="s">
@@ -6818,7 +6983,7 @@
       <c r="A47">
         <v>101</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" t="s">
         <v>179</v>
       </c>
       <c r="C47" t="s">
@@ -6858,7 +7023,7 @@
       <c r="A48">
         <v>102</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B48" t="s">
         <v>181</v>
       </c>
       <c r="C48" t="s">
@@ -6899,7 +7064,7 @@
       <c r="A49">
         <v>102</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" t="s">
         <v>181</v>
       </c>
       <c r="C49" t="s">
@@ -6940,7 +7105,7 @@
       <c r="A50">
         <v>106</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" t="s">
         <v>220</v>
       </c>
       <c r="C50" t="s">
@@ -6981,7 +7146,7 @@
       <c r="A51">
         <v>104</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B51" t="s">
         <v>183</v>
       </c>
       <c r="C51" t="s">
@@ -7022,7 +7187,7 @@
       <c r="A52">
         <v>104</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" t="s">
         <v>183</v>
       </c>
       <c r="C52" t="s">
@@ -7063,7 +7228,7 @@
       <c r="A53">
         <v>102</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" t="s">
         <v>181</v>
       </c>
       <c r="C53" t="s">
@@ -7118,7 +7283,7 @@
       <c r="A54">
         <v>102</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B54" t="s">
         <v>181</v>
       </c>
       <c r="C54" t="s">
@@ -7173,7 +7338,7 @@
       <c r="A55">
         <v>104</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" t="s">
         <v>183</v>
       </c>
       <c r="C55" t="s">
@@ -7214,7 +7379,7 @@
       <c r="A56">
         <v>104</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B56" t="s">
         <v>183</v>
       </c>
       <c r="C56" t="s">
@@ -7255,7 +7420,7 @@
       <c r="A57">
         <v>107</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="B57" t="s">
         <v>246</v>
       </c>
       <c r="C57" t="s">
@@ -7296,7 +7461,7 @@
       <c r="A58">
         <v>106</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B58" t="s">
         <v>220</v>
       </c>
       <c r="C58" t="s">
@@ -7337,7 +7502,7 @@
       <c r="A59">
         <v>107</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B59" t="s">
         <v>246</v>
       </c>
       <c r="C59" t="s">
@@ -7378,7 +7543,7 @@
       <c r="A60">
         <v>106</v>
       </c>
-      <c r="B60" s="8" t="s">
+      <c r="B60" t="s">
         <v>220</v>
       </c>
       <c r="C60" t="s">
@@ -7419,7 +7584,7 @@
       <c r="A61">
         <v>107</v>
       </c>
-      <c r="B61" s="8" t="s">
+      <c r="B61" t="s">
         <v>246</v>
       </c>
       <c r="C61" t="s">
@@ -7467,7 +7632,7 @@
       <c r="A62">
         <v>107</v>
       </c>
-      <c r="B62" s="8" t="s">
+      <c r="B62" t="s">
         <v>246</v>
       </c>
       <c r="C62" t="s">
@@ -7515,7 +7680,7 @@
       <c r="A63">
         <v>106</v>
       </c>
-      <c r="B63" s="8" t="s">
+      <c r="B63" t="s">
         <v>220</v>
       </c>
       <c r="C63" t="s">
@@ -7555,7 +7720,7 @@
       <c r="A64">
         <v>103</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="B64" t="s">
         <v>182</v>
       </c>
       <c r="C64" t="s">
@@ -7596,7 +7761,7 @@
       <c r="A65">
         <v>101</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="B65" t="s">
         <v>179</v>
       </c>
       <c r="C65" t="s">
@@ -7637,7 +7802,7 @@
       <c r="A66">
         <v>101</v>
       </c>
-      <c r="B66" s="8" t="s">
+      <c r="B66" t="s">
         <v>179</v>
       </c>
       <c r="C66" t="s">
@@ -7677,7 +7842,7 @@
       <c r="A67">
         <v>104</v>
       </c>
-      <c r="B67" s="8" t="s">
+      <c r="B67" t="s">
         <v>183</v>
       </c>
       <c r="C67" t="s">
@@ -7732,7 +7897,7 @@
       <c r="A68">
         <v>104</v>
       </c>
-      <c r="B68" s="8" t="s">
+      <c r="B68" t="s">
         <v>183</v>
       </c>
       <c r="C68" t="s">
@@ -7787,7 +7952,7 @@
       <c r="A69">
         <v>104</v>
       </c>
-      <c r="B69" s="8" t="s">
+      <c r="B69" t="s">
         <v>183</v>
       </c>
       <c r="C69" t="s">
@@ -7842,7 +8007,7 @@
       <c r="A70">
         <v>106</v>
       </c>
-      <c r="B70" s="8" t="s">
+      <c r="B70" t="s">
         <v>220</v>
       </c>
       <c r="C70" t="s">
@@ -7883,7 +8048,7 @@
       <c r="A71">
         <v>106</v>
       </c>
-      <c r="B71" s="8" t="s">
+      <c r="B71" t="s">
         <v>220</v>
       </c>
       <c r="C71" t="s">
@@ -7924,7 +8089,7 @@
       <c r="A72">
         <v>106</v>
       </c>
-      <c r="B72" s="8" t="s">
+      <c r="B72" t="s">
         <v>220</v>
       </c>
       <c r="C72" t="s">
@@ -7964,7 +8129,7 @@
       <c r="A73">
         <v>107</v>
       </c>
-      <c r="B73" s="8" t="s">
+      <c r="B73" t="s">
         <v>246</v>
       </c>
       <c r="C73" t="s">
@@ -8005,7 +8170,7 @@
       <c r="A74">
         <v>107</v>
       </c>
-      <c r="B74" s="8" t="s">
+      <c r="B74" t="s">
         <v>246</v>
       </c>
       <c r="C74" t="s">
@@ -8046,7 +8211,7 @@
       <c r="A75">
         <v>101</v>
       </c>
-      <c r="B75" s="8" t="s">
+      <c r="B75" t="s">
         <v>179</v>
       </c>
       <c r="C75" t="s">
@@ -8087,7 +8252,7 @@
       <c r="A76">
         <v>104</v>
       </c>
-      <c r="B76" s="8" t="s">
+      <c r="B76" t="s">
         <v>183</v>
       </c>
       <c r="C76" t="s">
@@ -8128,7 +8293,7 @@
       <c r="A77">
         <v>103</v>
       </c>
-      <c r="B77" s="8" t="s">
+      <c r="B77" t="s">
         <v>182</v>
       </c>
       <c r="C77" t="s">
@@ -8169,7 +8334,7 @@
       <c r="A78">
         <v>106</v>
       </c>
-      <c r="B78" s="8" t="s">
+      <c r="B78" t="s">
         <v>220</v>
       </c>
       <c r="C78" t="s">
@@ -8210,7 +8375,7 @@
       <c r="A79">
         <v>104</v>
       </c>
-      <c r="B79" s="8" t="s">
+      <c r="B79" t="s">
         <v>183</v>
       </c>
       <c r="C79" t="s">
@@ -8251,7 +8416,7 @@
       <c r="A80">
         <v>106</v>
       </c>
-      <c r="B80" s="8" t="s">
+      <c r="B80" t="s">
         <v>220</v>
       </c>
       <c r="C80" t="s">
@@ -8292,7 +8457,7 @@
       <c r="A81">
         <v>104</v>
       </c>
-      <c r="B81" s="8" t="s">
+      <c r="B81" t="s">
         <v>183</v>
       </c>
       <c r="C81" t="s">
@@ -8333,7 +8498,7 @@
       <c r="A82">
         <v>106</v>
       </c>
-      <c r="B82" s="8" t="s">
+      <c r="B82" t="s">
         <v>220</v>
       </c>
       <c r="C82" t="s">
@@ -8373,7 +8538,7 @@
       <c r="A83">
         <v>104</v>
       </c>
-      <c r="B83" s="8" t="s">
+      <c r="B83" t="s">
         <v>183</v>
       </c>
       <c r="C83" t="s">
@@ -8414,7 +8579,7 @@
       <c r="A84">
         <v>104</v>
       </c>
-      <c r="B84" s="8" t="s">
+      <c r="B84" t="s">
         <v>183</v>
       </c>
       <c r="C84" t="s">
@@ -8455,7 +8620,7 @@
       <c r="A85">
         <v>104</v>
       </c>
-      <c r="B85" s="8" t="s">
+      <c r="B85" t="s">
         <v>183</v>
       </c>
       <c r="C85" t="s">
@@ -8496,7 +8661,7 @@
       <c r="A86">
         <v>102</v>
       </c>
-      <c r="B86" s="8" t="s">
+      <c r="B86" t="s">
         <v>181</v>
       </c>
       <c r="C86" t="s">
@@ -8537,7 +8702,7 @@
       <c r="A87">
         <v>102</v>
       </c>
-      <c r="B87" s="8" t="s">
+      <c r="B87" t="s">
         <v>181</v>
       </c>
       <c r="C87" t="s">
@@ -8578,7 +8743,7 @@
       <c r="A88">
         <v>106</v>
       </c>
-      <c r="B88" s="8" t="s">
+      <c r="B88" t="s">
         <v>220</v>
       </c>
       <c r="C88" t="s">
@@ -8619,7 +8784,7 @@
       <c r="A89">
         <v>102</v>
       </c>
-      <c r="B89" s="8" t="s">
+      <c r="B89" t="s">
         <v>181</v>
       </c>
       <c r="C89" t="s">
@@ -8660,7 +8825,7 @@
       <c r="A90">
         <v>102</v>
       </c>
-      <c r="B90" s="8" t="s">
+      <c r="B90" t="s">
         <v>181</v>
       </c>
       <c r="C90" t="s">
@@ -8701,7 +8866,7 @@
       <c r="A91">
         <v>104</v>
       </c>
-      <c r="B91" s="8" t="s">
+      <c r="B91" t="s">
         <v>183</v>
       </c>
       <c r="C91" t="s">
@@ -8742,7 +8907,7 @@
       <c r="A92">
         <v>104</v>
       </c>
-      <c r="B92" s="8" t="s">
+      <c r="B92" t="s">
         <v>183</v>
       </c>
       <c r="C92" t="s">
@@ -8783,7 +8948,7 @@
       <c r="A93">
         <v>107</v>
       </c>
-      <c r="B93" s="8" t="s">
+      <c r="B93" t="s">
         <v>246</v>
       </c>
       <c r="C93" t="s">
@@ -8824,7 +8989,7 @@
       <c r="A94">
         <v>104</v>
       </c>
-      <c r="B94" s="8" t="s">
+      <c r="B94" t="s">
         <v>183</v>
       </c>
       <c r="C94" t="s">
@@ -8865,7 +9030,7 @@
       <c r="A95">
         <v>106</v>
       </c>
-      <c r="B95" s="8" t="s">
+      <c r="B95" t="s">
         <v>220</v>
       </c>
       <c r="C95" t="s">
@@ -8906,7 +9071,7 @@
       <c r="A96">
         <v>107</v>
       </c>
-      <c r="B96" s="8" t="s">
+      <c r="B96" t="s">
         <v>246</v>
       </c>
       <c r="C96" t="s">
@@ -8947,7 +9112,7 @@
       <c r="A97">
         <v>106</v>
       </c>
-      <c r="B97" s="8" t="s">
+      <c r="B97" t="s">
         <v>220</v>
       </c>
       <c r="C97" t="s">
@@ -8988,7 +9153,7 @@
       <c r="A98">
         <v>107</v>
       </c>
-      <c r="B98" s="8" t="s">
+      <c r="B98" t="s">
         <v>246</v>
       </c>
       <c r="C98" t="s">
@@ -9036,7 +9201,7 @@
       <c r="A99">
         <v>107</v>
       </c>
-      <c r="B99" s="8" t="s">
+      <c r="B99" t="s">
         <v>246</v>
       </c>
       <c r="C99" t="s">
@@ -9084,7 +9249,7 @@
       <c r="A100">
         <v>106</v>
       </c>
-      <c r="B100" s="8" t="s">
+      <c r="B100" t="s">
         <v>220</v>
       </c>
       <c r="C100" t="s">
@@ -9124,7 +9289,7 @@
       <c r="A101">
         <v>103</v>
       </c>
-      <c r="B101" s="8" t="s">
+      <c r="B101" t="s">
         <v>182</v>
       </c>
       <c r="C101" t="s">
@@ -9165,7 +9330,7 @@
       <c r="A102">
         <v>101</v>
       </c>
-      <c r="B102" s="8" t="s">
+      <c r="B102" t="s">
         <v>179</v>
       </c>
       <c r="C102" t="s">
@@ -9206,7 +9371,7 @@
       <c r="A103">
         <v>101</v>
       </c>
-      <c r="B103" s="8" t="s">
+      <c r="B103" t="s">
         <v>179</v>
       </c>
       <c r="C103" t="s">
@@ -9246,7 +9411,7 @@
       <c r="A104">
         <v>106</v>
       </c>
-      <c r="B104" s="8" t="s">
+      <c r="B104" t="s">
         <v>220</v>
       </c>
       <c r="C104" t="s">
@@ -9287,7 +9452,7 @@
       <c r="A105">
         <v>104</v>
       </c>
-      <c r="B105" s="8" t="s">
+      <c r="B105" t="s">
         <v>183</v>
       </c>
       <c r="C105" t="s">
@@ -9342,7 +9507,7 @@
       <c r="A106">
         <v>104</v>
       </c>
-      <c r="B106" s="8" t="s">
+      <c r="B106" t="s">
         <v>183</v>
       </c>
       <c r="C106" t="s">
@@ -9397,7 +9562,7 @@
       <c r="A107">
         <v>104</v>
       </c>
-      <c r="B107" s="8" t="s">
+      <c r="B107" t="s">
         <v>183</v>
       </c>
       <c r="C107" t="s">
@@ -9452,7 +9617,7 @@
       <c r="A108">
         <v>106</v>
       </c>
-      <c r="B108" s="8" t="s">
+      <c r="B108" t="s">
         <v>220</v>
       </c>
       <c r="C108" t="s">
@@ -9493,7 +9658,7 @@
       <c r="A109">
         <v>106</v>
       </c>
-      <c r="B109" s="8" t="s">
+      <c r="B109" t="s">
         <v>220</v>
       </c>
       <c r="C109" t="s">
@@ -9533,7 +9698,7 @@
       <c r="A110">
         <v>107</v>
       </c>
-      <c r="B110" s="8" t="s">
+      <c r="B110" t="s">
         <v>246</v>
       </c>
       <c r="C110" t="s">
@@ -9574,7 +9739,7 @@
       <c r="A111">
         <v>107</v>
       </c>
-      <c r="B111" s="8" t="s">
+      <c r="B111" t="s">
         <v>246</v>
       </c>
       <c r="C111" t="s">
@@ -9615,7 +9780,7 @@
       <c r="A112">
         <v>107</v>
       </c>
-      <c r="B112" s="8" t="s">
+      <c r="B112" t="s">
         <v>246</v>
       </c>
       <c r="C112" t="s">
@@ -9656,7 +9821,7 @@
       <c r="A113">
         <v>107</v>
       </c>
-      <c r="B113" s="8" t="s">
+      <c r="B113" t="s">
         <v>246</v>
       </c>
       <c r="C113" t="s">
@@ -9697,7 +9862,7 @@
       <c r="A114">
         <v>101</v>
       </c>
-      <c r="B114" s="8" t="s">
+      <c r="B114" t="s">
         <v>179</v>
       </c>
       <c r="C114" t="s">
@@ -9738,7 +9903,7 @@
       <c r="A115">
         <v>103</v>
       </c>
-      <c r="B115" s="8" t="s">
+      <c r="B115" t="s">
         <v>182</v>
       </c>
       <c r="C115" t="s">
@@ -9779,7 +9944,7 @@
       <c r="A116">
         <v>104</v>
       </c>
-      <c r="B116" s="8" t="s">
+      <c r="B116" t="s">
         <v>183</v>
       </c>
       <c r="C116" t="s">
@@ -9820,7 +9985,7 @@
       <c r="A117">
         <v>106</v>
       </c>
-      <c r="B117" s="8" t="s">
+      <c r="B117" t="s">
         <v>220</v>
       </c>
       <c r="C117" t="s">
@@ -9861,7 +10026,7 @@
       <c r="A118">
         <v>106</v>
       </c>
-      <c r="B118" s="8" t="s">
+      <c r="B118" t="s">
         <v>220</v>
       </c>
       <c r="C118" t="s">
@@ -9902,7 +10067,7 @@
       <c r="A119">
         <v>104</v>
       </c>
-      <c r="B119" s="8" t="s">
+      <c r="B119" t="s">
         <v>183</v>
       </c>
       <c r="C119" t="s">
@@ -9943,7 +10108,7 @@
       <c r="A120">
         <v>104</v>
       </c>
-      <c r="B120" s="8" t="s">
+      <c r="B120" t="s">
         <v>183</v>
       </c>
       <c r="C120" t="s">
@@ -9984,7 +10149,7 @@
       <c r="A121">
         <v>104</v>
       </c>
-      <c r="B121" s="8" t="s">
+      <c r="B121" t="s">
         <v>183</v>
       </c>
       <c r="C121" t="s">
@@ -10025,7 +10190,7 @@
       <c r="A122">
         <v>106</v>
       </c>
-      <c r="B122" s="8" t="s">
+      <c r="B122" t="s">
         <v>220</v>
       </c>
       <c r="C122" t="s">
@@ -10065,7 +10230,7 @@
       <c r="A123">
         <v>104</v>
       </c>
-      <c r="B123" s="8" t="s">
+      <c r="B123" t="s">
         <v>183</v>
       </c>
       <c r="C123" t="s">
@@ -10106,7 +10271,7 @@
       <c r="A124">
         <v>104</v>
       </c>
-      <c r="B124" s="8" t="s">
+      <c r="B124" t="s">
         <v>183</v>
       </c>
       <c r="C124" t="s">
@@ -10147,7 +10312,7 @@
       <c r="A125">
         <v>102</v>
       </c>
-      <c r="B125" s="8" t="s">
+      <c r="B125" t="s">
         <v>181</v>
       </c>
       <c r="C125" t="s">
@@ -10188,7 +10353,7 @@
       <c r="A126">
         <v>102</v>
       </c>
-      <c r="B126" s="8" t="s">
+      <c r="B126" t="s">
         <v>181</v>
       </c>
       <c r="C126" t="s">
@@ -10229,7 +10394,7 @@
       <c r="A127">
         <v>102</v>
       </c>
-      <c r="B127" s="8" t="s">
+      <c r="B127" t="s">
         <v>181</v>
       </c>
       <c r="C127" t="s">
@@ -10270,7 +10435,7 @@
       <c r="A128">
         <v>102</v>
       </c>
-      <c r="B128" s="8" t="s">
+      <c r="B128" t="s">
         <v>181</v>
       </c>
       <c r="C128" t="s">
@@ -10311,7 +10476,7 @@
       <c r="A129">
         <v>106</v>
       </c>
-      <c r="B129" s="8" t="s">
+      <c r="B129" t="s">
         <v>220</v>
       </c>
       <c r="C129" t="s">
@@ -10352,7 +10517,7 @@
       <c r="A130">
         <v>104</v>
       </c>
-      <c r="B130" s="8" t="s">
+      <c r="B130" t="s">
         <v>183</v>
       </c>
       <c r="C130" t="s">
@@ -10393,7 +10558,7 @@
       <c r="A131">
         <v>104</v>
       </c>
-      <c r="B131" s="8" t="s">
+      <c r="B131" t="s">
         <v>183</v>
       </c>
       <c r="C131" t="s">
@@ -10434,7 +10599,7 @@
       <c r="A132">
         <v>102</v>
       </c>
-      <c r="B132" s="8" t="s">
+      <c r="B132" t="s">
         <v>181</v>
       </c>
       <c r="C132" t="s">
@@ -10489,7 +10654,7 @@
       <c r="A133">
         <v>102</v>
       </c>
-      <c r="B133" s="8" t="s">
+      <c r="B133" t="s">
         <v>181</v>
       </c>
       <c r="C133" t="s">
@@ -10544,7 +10709,7 @@
       <c r="A134">
         <v>107</v>
       </c>
-      <c r="B134" s="8" t="s">
+      <c r="B134" t="s">
         <v>246</v>
       </c>
       <c r="C134" t="s">
@@ -10585,7 +10750,7 @@
       <c r="A135">
         <v>106</v>
       </c>
-      <c r="B135" s="8" t="s">
+      <c r="B135" t="s">
         <v>220</v>
       </c>
       <c r="C135" t="s">
@@ -10626,7 +10791,7 @@
       <c r="A136">
         <v>107</v>
       </c>
-      <c r="B136" s="8" t="s">
+      <c r="B136" t="s">
         <v>246</v>
       </c>
       <c r="C136" t="s">
@@ -10667,7 +10832,7 @@
       <c r="A137">
         <v>104</v>
       </c>
-      <c r="B137" s="8" t="s">
+      <c r="B137" t="s">
         <v>183</v>
       </c>
       <c r="C137" t="s">
@@ -10708,7 +10873,7 @@
       <c r="A138">
         <v>106</v>
       </c>
-      <c r="B138" s="8" t="s">
+      <c r="B138" t="s">
         <v>220</v>
       </c>
       <c r="C138" t="s">
@@ -10749,7 +10914,7 @@
       <c r="A139">
         <v>107</v>
       </c>
-      <c r="B139" s="8" t="s">
+      <c r="B139" t="s">
         <v>246</v>
       </c>
       <c r="C139" t="s">
@@ -10797,7 +10962,7 @@
       <c r="A140">
         <v>107</v>
       </c>
-      <c r="B140" s="8" t="s">
+      <c r="B140" t="s">
         <v>246</v>
       </c>
       <c r="C140" t="s">
@@ -10845,7 +11010,7 @@
       <c r="A141">
         <v>103</v>
       </c>
-      <c r="B141" s="8" t="s">
+      <c r="B141" t="s">
         <v>182</v>
       </c>
       <c r="C141" t="s">
@@ -10899,21 +11064,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E2F6ACCA1C4E9E429EC0979D7AA69E5C" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ae8745856df04360dd1be451017c997c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="caec8013-4252-46d5-9263-a99cc59dead2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a5f7786c0b3d9081a77d0462e727a0e9" ns2:_="">
     <xsd:import namespace="caec8013-4252-46d5-9263-a99cc59dead2"/>
@@ -11051,31 +11201,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA37870F-1997-46E6-ABF3-D972D5619E05}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="caec8013-4252-46d5-9263-a99cc59dead2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E8E74F1-259B-4A8D-986B-B2E55FA52FD9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C42AE87-F6E1-4C18-815A-DDBC6D0FAC4D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11091,4 +11232,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E8E74F1-259B-4A8D-986B-B2E55FA52FD9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA37870F-1997-46E6-ABF3-D972D5619E05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="caec8013-4252-46d5-9263-a99cc59dead2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>